<commit_message>
Präsi, upd backlog & bd chart
</commit_message>
<xml_diff>
--- a/doc/CS1/task10/scrum_v02.xlsx
+++ b/doc/CS1/task10/scrum_v02.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se_000\Documents\GitHub\ch.bfh.bti7081.s2017.red\doc\CS1\task10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Git\ch.bfh.bti7081.s2017.red\doc\CS1\task10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="300" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -241,12 +241,33 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Open?</t>
+  </si>
+  <si>
+    <t>Partially Done (80%)</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>UI Ready needs extension, Logic started, overall 75%</t>
+  </si>
+  <si>
+    <t>UI Ready, bakend connection nyi, overall 50%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,7 +285,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +304,24 @@
         <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -296,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,9 +358,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -402,6 +454,987 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Remaining Effort</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>42857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>235</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Remaining Resources</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>42857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="410512344"/>
+        <c:axId val="410510704"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="410512344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410510704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="410510704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410512344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>168274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>279399</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>69849</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4509BF8-FDB2-49A6-92D3-5A1113511C84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,17 +1703,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="15.36328125"/>
+    <col min="2" max="2" width="16.6328125"/>
+    <col min="3" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +1724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -702,7 +1735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -713,7 +1746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -724,7 +1757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -735,7 +1768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -757,23 +1790,23 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="2"/>
-    <col min="2" max="2" width="35.44140625" style="2"/>
-    <col min="3" max="3" width="44.5546875" style="3"/>
-    <col min="4" max="4" width="8.44140625"/>
-    <col min="5" max="5" width="11.6640625"/>
-    <col min="6" max="6" width="13.109375"/>
-    <col min="7" max="7" width="10.109375"/>
-    <col min="8" max="8" width="15.6640625"/>
-    <col min="9" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="3.6328125" style="2"/>
+    <col min="2" max="2" width="35.453125" style="2"/>
+    <col min="3" max="3" width="44.54296875" style="3"/>
+    <col min="4" max="4" width="8.453125"/>
+    <col min="5" max="5" width="11.6328125"/>
+    <col min="6" max="6" width="13.08984375"/>
+    <col min="7" max="7" width="10.08984375"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="9" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -799,7 +1832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -815,15 +1848,18 @@
       <c r="E2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
@@ -832,8 +1868,11 @@
       <c r="E3">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -849,8 +1888,11 @@
       <c r="E4">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H4" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -866,8 +1908,11 @@
       <c r="E5">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H5" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -883,8 +1928,11 @@
       <c r="E6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -900,8 +1948,11 @@
       <c r="E7">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E19">
         <f>SUM(E2:E13)</f>
         <v>270</v>
@@ -913,7 +1964,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -922,27 +1973,27 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.6640625"/>
-    <col min="2" max="2" width="6.33203125"/>
-    <col min="3" max="3" width="29.88671875"/>
-    <col min="4" max="4" width="50.109375"/>
-    <col min="5" max="5" width="19.6640625"/>
-    <col min="6" max="6" width="11.6640625"/>
-    <col min="7" max="7" width="9.6640625"/>
-    <col min="8" max="8" width="8.33203125"/>
-    <col min="9" max="9" width="7.88671875"/>
-    <col min="10" max="10" width="9.109375"/>
-    <col min="11" max="11" width="7.33203125"/>
-    <col min="12" max="12" width="15.33203125"/>
-    <col min="13" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="4.6328125"/>
+    <col min="2" max="2" width="6.36328125"/>
+    <col min="3" max="3" width="29.90625"/>
+    <col min="4" max="4" width="51.36328125" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125"/>
+    <col min="6" max="6" width="11.6328125"/>
+    <col min="7" max="7" width="9.6328125"/>
+    <col min="8" max="8" width="8.36328125"/>
+    <col min="9" max="9" width="7.90625"/>
+    <col min="10" max="10" width="9.08984375"/>
+    <col min="11" max="11" width="7.36328125"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -980,286 +2031,318 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="8">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8">
+        <v>4</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
         <v>1.4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="10">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="J3" s="10"/>
+      <c r="K3" s="10">
+        <v>6</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
         <v>1.2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="8">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
         <v>1.3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="10">
         <v>4</v>
       </c>
-      <c r="L5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="J5" s="10"/>
+      <c r="K5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
         <v>0.1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="8">
         <v>2</v>
       </c>
-      <c r="L6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
         <v>1.4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="8">
         <v>8</v>
       </c>
-      <c r="L7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8">
+        <v>4</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
         <v>2.1</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="8">
         <v>4</v>
       </c>
-      <c r="L8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="9">
         <v>8</v>
       </c>
-      <c r="L9" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5546875"/>
-    <col min="2" max="2" width="13.109375"/>
-    <col min="3" max="3" width="14.6640625"/>
-    <col min="4" max="4" width="14.33203125"/>
-    <col min="5" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="8.54296875"/>
+    <col min="2" max="2" width="13.08984375"/>
+    <col min="3" max="3" width="14.6328125"/>
+    <col min="4" max="4" width="14.36328125"/>
+    <col min="5" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -1273,36 +2356,66 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>42262</v>
+        <v>42857</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="D2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>42263</v>
+        <v>42866</v>
       </c>
       <c r="C3">
-        <v>190</v>
+        <f>C2-35</f>
+        <v>235</v>
       </c>
       <c r="D3">
-        <v>180</v>
-      </c>
+        <f>D2-34</f>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upd präsi, sprint 02 backlog
</commit_message>
<xml_diff>
--- a/doc/CS1/task10/scrum_v02.xlsx
+++ b/doc/CS1/task10/scrum_v02.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="300" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="300" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint Backlog S1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint Backlog S2" sheetId="5" r:id="rId4"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -243,18 +244,9 @@
     <t>All</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
-    <t>Open?</t>
-  </si>
-  <si>
-    <t>Partially Done (80%)</t>
-  </si>
-  <si>
     <t>Not started</t>
   </si>
   <si>
@@ -262,13 +254,70 @@
   </si>
   <si>
     <t>UI Ready, bakend connection nyi, overall 50%</t>
+  </si>
+  <si>
+    <t>Sprint  1: 7 h. p.P.</t>
+  </si>
+  <si>
+    <t>Total Sprint 1</t>
+  </si>
+  <si>
+    <t>Domain Model</t>
+  </si>
+  <si>
+    <t>All persistent data as chart and implemented (Task 12, due 26.05.17)</t>
+  </si>
+  <si>
+    <t>Patient states</t>
+  </si>
+  <si>
+    <t>Timetable</t>
+  </si>
+  <si>
+    <t>Basic View and implementation: Add Event / Session, overview</t>
+  </si>
+  <si>
+    <t>Left over from Sprint 1</t>
+  </si>
+  <si>
+    <t>New Features Sprint 2</t>
+  </si>
+  <si>
+    <t>Patient can have different states (Task 13) which define Doctor's tasks</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Encyption and persistence of passwords</t>
+  </si>
+  <si>
+    <t>Main View redesign</t>
+  </si>
+  <si>
+    <t>Buttons by graphics, Buttons on top, Mobile ability</t>
+  </si>
+  <si>
+    <t>Patient Search</t>
+  </si>
+  <si>
+    <t>Implement View, Filtering request (XML/JSON), load to patient view</t>
+  </si>
+  <si>
+    <t>UI/view/db</t>
+  </si>
+  <si>
+    <t>Services add, remove, filter operations</t>
+  </si>
+  <si>
+    <t>Ali/Rolf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,8 +333,30 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,12 +389,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -331,11 +408,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,16 +503,8 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -371,11 +512,42 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -579,7 +751,7 @@
                   <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>235</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -634,7 +806,7 @@
                   <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1703,7 +1875,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1848,8 +2020,8 @@
       <c r="E2">
         <v>34</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>78</v>
+      <c r="H2" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1859,7 +2031,7 @@
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
@@ -1868,8 +2040,8 @@
       <c r="E3">
         <v>32</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>79</v>
+      <c r="H3" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1888,8 +2060,8 @@
       <c r="E4">
         <v>32</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1908,8 +2080,8 @@
       <c r="E5">
         <v>32</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>77</v>
+      <c r="H5" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -1928,8 +2100,8 @@
       <c r="E6">
         <v>60</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>77</v>
+      <c r="H6" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1948,8 +2120,8 @@
       <c r="E7">
         <v>80</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>77</v>
+      <c r="H7" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.35">
@@ -1970,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1993,7 +2165,7 @@
     <col min="13" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2031,295 +2203,333 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="6">
         <v>12</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6">
         <v>4</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
+      <c r="L2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="6">
+        <f>IF(L2="Done",I2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
         <v>1.4</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <v>8</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="7">
+        <f t="shared" ref="M3:M9" si="0">IF(L3="Done",I3,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7">
+        <v>8</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="7">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7">
+        <v>3</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="6">
+        <v>8</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6">
+        <v>4</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I8" s="7">
+        <v>4</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="13">
         <v>8</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8">
-        <v>3</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>1.3</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="10">
-        <v>4</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="8">
-        <v>2</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8">
-        <v>1</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
-        <v>1.4</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="8">
-        <v>8</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8">
-        <v>4</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
-        <v>2.1</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="8">
-        <v>4</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8">
-        <v>2</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B9" s="9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="9">
-        <v>8</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9">
-        <v>4</v>
-      </c>
-      <c r="L9" s="9" t="s">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13" t="s">
         <v>45</v>
       </c>
+      <c r="M9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="14">
+        <f>SUM(M2:M9)</f>
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:M2">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>"L2=""Open"""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2327,91 +2537,965 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.54296875"/>
-    <col min="2" max="2" width="13.08984375"/>
-    <col min="3" max="3" width="14.6328125"/>
-    <col min="4" max="4" width="14.36328125"/>
-    <col min="5" max="1025" width="8.54296875"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="15">
+        <v>8</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="15">
+        <f t="shared" ref="M3:M16" si="0">IF(L3="Done",I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="15">
+        <f>IF(IFERROR(SEARCH(P$2,$F3),FALSE),$I3,0)</f>
+        <v>8</v>
+      </c>
+      <c r="Q3" s="15">
+        <f t="shared" ref="Q3:T3" si="1">IF(IFERROR(SEARCH(Q$2,$F3),FALSE),$I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S3" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T3" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="15">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="15">
+        <v>8</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="15">
+        <f t="shared" ref="P4:T16" si="2">IF(IFERROR(SEARCH(P$2,$F4),FALSE),$I4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="T4" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="15">
+        <v>4</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="T5" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="18"/>
+      <c r="P6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="B7" s="15">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="15">
+        <v>4</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="S7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="15">
+        <v>8</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="S8" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15">
+        <v>16</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="B10" s="15">
+        <v>2</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
+        <v>8</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
+        <v>4</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="B12" s="15">
+        <v>2</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
+        <v>8</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>4</v>
+      </c>
+      <c r="R12" s="15">
+        <v>4</v>
+      </c>
+      <c r="S12" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="B13" s="15">
+        <v>2</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15">
+        <v>8</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="R13" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="B14" s="15">
+        <v>2</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15">
+        <v>8</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="T14" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="B15" s="15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="8:20" x14ac:dyDescent="0.35">
+      <c r="H17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="15">
+        <f>SUM(I3:I5)+SUM(I7:I16)</f>
+        <v>84</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="15">
+        <f>SUM(M3:M5)+SUM(M7:M16)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="P17" s="15">
+        <f>SUM(P3:P16)</f>
+        <v>8</v>
+      </c>
+      <c r="Q17" s="15">
+        <f t="shared" ref="Q17:T17" si="3">SUM(Q3:Q16)</f>
+        <v>16</v>
+      </c>
+      <c r="R17" s="15">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S17" s="15">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T17" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A2:M2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="P3:T16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.54296875" style="11"/>
+    <col min="2" max="2" width="13.08984375" style="11"/>
+    <col min="3" max="3" width="14.6328125" style="11"/>
+    <col min="4" max="4" width="14.36328125" style="11"/>
+    <col min="5" max="1025" width="8.54296875" style="11"/>
+    <col min="1026" max="16384" width="8.90625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="12">
         <v>42857</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>270</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="11">
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="12">
         <v>42866</v>
       </c>
-      <c r="C3">
-        <f>C2-35</f>
-        <v>235</v>
-      </c>
-      <c r="D3">
-        <f>D2-34</f>
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
+      <c r="C3" s="11">
+        <f>C2-'Sprint Backlog S1'!M10</f>
+        <v>248</v>
+      </c>
+      <c r="D3" s="11">
+        <f>D2-37</f>
+        <v>233</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added exception handeling to user login, started to implement password security
</commit_message>
<xml_diff>
--- a/doc/CS1/task10/scrum_v02.xlsx
+++ b/doc/CS1/task10/scrum_v02.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Git\ch.bfh.bti7081.s2017.red\doc\CS1\task10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rolf/GitHub/Semester4/ch.bfh.bti7081.s2017.red/doc/CS1/task10/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="300" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" tabRatio="300" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,20 @@
     <sheet name="Sprint Backlog S2" sheetId="5" r:id="rId4"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -323,12 +331,18 @@
   </si>
   <si>
     <t>More!!!!!</t>
+  </si>
+  <si>
+    <t>Adrian/Flo</t>
+  </si>
+  <si>
+    <t>opt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,29 +436,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -452,34 +466,34 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,7 +502,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,6 +546,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,9 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +658,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -713,7 +727,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -745,13 +759,13 @@
             <c:numRef>
               <c:f>BurndownChart!$B$2:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>42857</c:v>
+                  <c:v>42857.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42866</c:v>
+                  <c:v>42866.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -763,16 +777,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>248</c:v>
+                  <c:v>248.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
             </c:ext>
@@ -800,13 +814,13 @@
             <c:numRef>
               <c:f>BurndownChart!$B$2:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>42857</c:v>
+                  <c:v>42857.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42866</c:v>
+                  <c:v>42866.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,16 +832,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233</c:v>
+                  <c:v>233.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
             </c:ext>
@@ -842,17 +856,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="410512344"/>
-        <c:axId val="410510704"/>
+        <c:axId val="1498477920"/>
+        <c:axId val="1498564768"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="410512344"/>
+        <c:axId val="1498477920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -886,17 +900,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410510704"/>
+        <c:crossAx val="1498564768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="410510704"/>
+        <c:axId val="1498564768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,10 +958,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410512344"/>
+        <c:crossAx val="1498477920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -986,7 +1000,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1016,7 +1030,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1603,7 +1617,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4509BF8-FDB2-49A6-92D3-5A1113511C84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4509BF8-FDB2-49A6-92D3-5A1113511C84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,18 +1903,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.36328125"/>
-    <col min="2" max="2" width="16.6328125"/>
-    <col min="3" max="1025" width="8.54296875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1922,7 +1931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1955,7 +1964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1976,24 +1985,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" style="2"/>
-    <col min="2" max="2" width="35.453125" style="2"/>
-    <col min="3" max="3" width="44.54296875" style="3"/>
-    <col min="4" max="4" width="8.453125"/>
-    <col min="5" max="5" width="11.6328125"/>
-    <col min="6" max="6" width="13.08984375"/>
-    <col min="7" max="7" width="10.08984375"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
-    <col min="9" max="1025" width="8.54296875"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="3" max="3" width="8.83203125" style="3"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="210" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="285" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E19">
         <f>SUM(E2:E13)</f>
         <v>270</v>
@@ -2159,28 +2162,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.6328125"/>
-    <col min="2" max="2" width="6.36328125"/>
-    <col min="3" max="3" width="29.90625"/>
-    <col min="4" max="4" width="51.36328125" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125"/>
-    <col min="6" max="6" width="11.6328125"/>
-    <col min="7" max="7" width="9.6328125"/>
-    <col min="8" max="8" width="8.36328125"/>
-    <col min="9" max="9" width="7.90625"/>
-    <col min="10" max="10" width="9.08984375"/>
-    <col min="11" max="11" width="7.36328125"/>
-    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.54296875"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2218,7 +2210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -2258,7 +2250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1.4</v>
       </c>
@@ -2296,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>1.2</v>
       </c>
@@ -2334,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>1.3</v>
       </c>
@@ -2374,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>0.1</v>
       </c>
@@ -2414,7 +2406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1.4</v>
       </c>
@@ -2454,7 +2446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>2.1</v>
       </c>
@@ -2492,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>2.2000000000000002</v>
       </c>
@@ -2530,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L10" s="14" t="s">
         <v>78</v>
       </c>
@@ -2554,19 +2546,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2604,22 +2596,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
       <c r="P2" s="4" t="s">
         <v>11</v>
       </c>
@@ -2636,7 +2628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1.4</v>
       </c>
@@ -2694,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>1.2</v>
       </c>
@@ -2752,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>1.3</v>
       </c>
@@ -2810,22 +2802,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
       <c r="P6" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2847,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>2.1</v>
       </c>
@@ -2905,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>2.2000000000000002</v>
       </c>
@@ -2963,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>2.2999999999999998</v>
       </c>
@@ -2977,9 +2969,13 @@
         <v>80</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="I9" s="15">
         <v>16</v>
       </c>
@@ -2994,7 +2990,7 @@
       </c>
       <c r="P9" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q9" s="15">
         <f t="shared" si="2"/>
@@ -3013,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>2.4</v>
       </c>
@@ -3027,7 +3023,9 @@
         <v>86</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15">
@@ -3044,7 +3042,7 @@
       </c>
       <c r="P10" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="15">
         <f t="shared" si="2"/>
@@ -3063,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>2.5</v>
       </c>
@@ -3117,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>2.6</v>
       </c>
@@ -3169,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>2.7</v>
       </c>
@@ -3223,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>2.8</v>
       </c>
@@ -3277,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>2.9</v>
       </c>
@@ -3331,8 +3329,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B16" s="15">
@@ -3377,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3417,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H18" s="15" t="s">
         <v>87</v>
       </c>
@@ -3437,7 +3435,7 @@
       </c>
       <c r="P18" s="15">
         <f>SUM(P3:P17)</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="Q18" s="15">
         <f t="shared" ref="Q18:T18" si="3">SUM(Q3:Q17)</f>
@@ -3480,21 +3478,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" style="11"/>
-    <col min="2" max="2" width="13.08984375" style="11"/>
-    <col min="3" max="3" width="14.6328125" style="11"/>
-    <col min="4" max="4" width="14.36328125" style="11"/>
-    <col min="5" max="1025" width="8.54296875" style="11"/>
-    <col min="1026" max="16384" width="8.90625" style="11"/>
+    <col min="1" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>64</v>
       </c>
@@ -3508,7 +3501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -3522,7 +3515,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -3541,31 +3534,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "scrum file update"
This reverts commit 7e7aef48a62a02c320d0fead3c0ac033d1ee9306.
</commit_message>
<xml_diff>
--- a/doc/CS1/task10/scrum_v02.xlsx
+++ b/doc/CS1/task10/scrum_v02.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Git\ch.bfh.bti7081.s2017.red\doc\CS1\task10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rolf/GitHub/Semester4/ch.bfh.bti7081.s2017.red/doc/CS1/task10/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" tabRatio="300" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" tabRatio="300" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint Backlog S2" sheetId="5" r:id="rId4"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -658,7 +658,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -727,7 +727,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -759,13 +759,13 @@
             <c:numRef>
               <c:f>BurndownChart!$B$2:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>42857</c:v>
+                  <c:v>42857.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42866</c:v>
+                  <c:v>42866.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,16 +777,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>248</c:v>
+                  <c:v>248.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
             </c:ext>
@@ -814,13 +814,13 @@
             <c:numRef>
               <c:f>BurndownChart!$B$2:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>42857</c:v>
+                  <c:v>42857.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42866</c:v>
+                  <c:v>42866.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -832,16 +832,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233</c:v>
+                  <c:v>233.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-89AA-4A1B-ACCC-B3A2C39C47E7}"/>
             </c:ext>
@@ -866,7 +866,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -900,7 +900,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1498564768"/>
@@ -958,7 +958,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1498477920"/>
@@ -1000,7 +1000,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1030,7 +1030,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1617,7 +1617,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4509BF8-FDB2-49A6-92D3-5A1113511C84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4509BF8-FDB2-49A6-92D3-5A1113511C84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1907,9 +1907,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1989,14 +1989,14 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.81640625" style="2"/>
-    <col min="3" max="3" width="8.81640625" style="3"/>
-    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="3" max="3" width="8.83203125" style="3"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="135" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="210" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="285" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E19">
         <f>SUM(E2:E13)</f>
         <v>270</v>
@@ -2162,17 +2162,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="51.36328125" customWidth="1"/>
-    <col min="12" max="12" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1.4</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>1.2</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>1.3</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>0.1</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1.4</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>2.1</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>2.2000000000000002</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L10" s="14" t="s">
         <v>78</v>
       </c>
@@ -2546,19 +2546,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>84</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1.4</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>1.2</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>1.3</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>85</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>2.1</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>2.2000000000000002</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>2.2999999999999998</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>2.4</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>2.5</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>2.6</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>2.7</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>2.8</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>2.9</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>96</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3415,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H18" s="15" t="s">
         <v>87</v>
       </c>
@@ -3482,12 +3482,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.81640625" style="11"/>
+    <col min="1" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>64</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -3534,31 +3534,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
     </row>
   </sheetData>

</xml_diff>